<commit_message>
general fix for namedRegion
</commit_message>
<xml_diff>
--- a/inst/extdata/namedRegions3.xlsx
+++ b/inst/extdata/namedRegions3.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" name="MyRange" vbProcedure="false">Sheet2!$A$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="MyRange" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="MyRange" vbProcedure="false">Sheet3!$A$1:$B$1</definedName>
   </definedNames>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">S1A1</t>
   </si>
@@ -37,13 +39,19 @@
     <t xml:space="preserve">S2A1</t>
   </si>
   <si>
-    <t xml:space="preserve">S2A2</t>
+    <t xml:space="preserve">S2B1</t>
   </si>
   <si>
     <t xml:space="preserve">S3A1</t>
   </si>
   <si>
     <t xml:space="preserve">S3B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4B1</t>
   </si>
 </sst>
 </file>
@@ -150,7 +158,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -182,13 +190,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -210,11 +218,11 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -233,4 +241,36 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1. check the sheets 2. check the named regions 3. remove unwanted named regions 4.1 if sheet is selected: keep only this sheet 4.2 if no sheet is selected: keep first sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/namedRegions3.xlsx
+++ b/inst/extdata/namedRegions3.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet0" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="MyRange" vbProcedure="false">Sheet2!$A$1:$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="MyRange" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="MyRange" vbProcedure="false">Sheet3!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="MyRange" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="MyRange" vbProcedure="false">Sheet3!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">S0A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S0B1</t>
+  </si>
   <si>
     <t xml:space="preserve">S1A1</t>
   </si>
@@ -154,18 +161,50 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -179,7 +218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -190,14 +229,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -211,7 +250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -222,14 +261,14 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -243,25 +282,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>7</v>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>